<commit_message>
productos importar, solo campos necesarios
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/f60_productos.xlsx
+++ b/assets/formatos_cargue/f60_productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Status</t>
   </si>
@@ -49,12 +49,6 @@
     <t>existencias</t>
   </si>
   <si>
-    <t>ID categoría</t>
-  </si>
-  <si>
-    <t>ID tipo</t>
-  </si>
-  <si>
     <t>Costo</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>K4GEST</t>
   </si>
   <si>
-    <t>ID Kit</t>
-  </si>
-  <si>
     <t>Nivel</t>
   </si>
   <si>
@@ -92,6 +83,9 @@
   </si>
   <si>
     <t>5,41,431</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -153,15 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -486,176 +477,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="58" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="11.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="33" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="58" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="33" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1">
+        <v>55000</v>
+      </c>
+      <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="I2" s="1">
+        <v>77000</v>
+      </c>
+      <c r="J2" s="1">
+        <v>320</v>
+      </c>
+      <c r="O2" s="1">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="P2" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1">
+        <v>89000</v>
+      </c>
+      <c r="O3" s="1">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>19</v>
+      <c r="P3" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1111</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1">
-        <v>55000</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>77000</v>
-      </c>
-      <c r="K2" s="1">
-        <v>320</v>
-      </c>
-      <c r="P2" s="1">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>4</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1111</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1">
-        <v>45000</v>
-      </c>
-      <c r="I3" s="1">
-        <v>19</v>
-      </c>
-      <c r="J3" s="1">
-        <v>89000</v>
-      </c>
-      <c r="P3" s="1">
-        <v>78</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>5</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="F4" s="8"/>
+    <row r="4" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>